<commit_message>
Changing gamma Including legend
</commit_message>
<xml_diff>
--- a/Citations for O'Hagan.xlsx
+++ b/Citations for O'Hagan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smp21js\Documents\R Projects\PhD-Materials\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamesalsbury/R Projects/PhD-Materials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48FAADC6-64FD-4B79-B173-2D3F20F115F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB7872DF-CEF8-2D4F-BBF1-E40A2E689CD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="24840" windowHeight="13280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -1887,23 +1887,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D4" zoomScale="89" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+    <sheetView tabSelected="1" topLeftCell="C83" zoomScale="89" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="C91" sqref="C91"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="3" max="3" width="129.6328125" customWidth="1"/>
-    <col min="4" max="4" width="12.81640625" customWidth="1"/>
+    <col min="3" max="3" width="129.6640625" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" customWidth="1"/>
     <col min="5" max="5" width="7" customWidth="1"/>
-    <col min="6" max="6" width="7.81640625" customWidth="1"/>
-    <col min="7" max="7" width="28.81640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.83203125" customWidth="1"/>
+    <col min="7" max="7" width="28.83203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1926,7 +1926,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1949,7 +1949,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1972,7 +1972,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1995,7 +1995,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -2018,7 +2018,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -2041,7 +2041,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -2064,7 +2064,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -2087,7 +2087,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -2110,7 +2110,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -2133,7 +2133,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -2156,7 +2156,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -2179,7 +2179,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>340</v>
       </c>
@@ -2202,7 +2202,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -2225,7 +2225,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -2248,7 +2248,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -2271,7 +2271,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>5</v>
       </c>
@@ -2294,7 +2294,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>5</v>
       </c>
@@ -2317,7 +2317,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>5</v>
       </c>
@@ -2340,7 +2340,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>5</v>
       </c>
@@ -2363,7 +2363,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>5</v>
       </c>
@@ -2386,7 +2386,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>5</v>
       </c>
@@ -2409,7 +2409,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -2432,7 +2432,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>5</v>
       </c>
@@ -2455,7 +2455,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>5</v>
       </c>
@@ -2478,7 +2478,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>5</v>
       </c>
@@ -2501,7 +2501,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>5</v>
       </c>
@@ -2524,7 +2524,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>5</v>
       </c>
@@ -2547,7 +2547,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>5</v>
       </c>
@@ -2570,7 +2570,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>5</v>
       </c>
@@ -2593,7 +2593,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>5</v>
       </c>
@@ -2616,7 +2616,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
         <v>5</v>
       </c>
@@ -2639,7 +2639,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
         <v>5</v>
       </c>
@@ -2662,7 +2662,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
         <v>5</v>
       </c>
@@ -2685,7 +2685,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
         <v>5</v>
       </c>
@@ -2708,7 +2708,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
         <v>5</v>
       </c>
@@ -2731,7 +2731,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
         <v>5</v>
       </c>
@@ -2754,7 +2754,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
         <v>5</v>
       </c>
@@ -2777,7 +2777,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
         <v>5</v>
       </c>
@@ -2800,7 +2800,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
         <v>5</v>
       </c>
@@ -2823,7 +2823,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
         <v>5</v>
       </c>
@@ -2846,7 +2846,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
         <v>5</v>
       </c>
@@ -2869,7 +2869,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
         <v>5</v>
       </c>
@@ -2892,7 +2892,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A44" t="s">
         <v>5</v>
       </c>
@@ -2915,7 +2915,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A45" t="s">
         <v>5</v>
       </c>
@@ -2938,7 +2938,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A46" t="s">
         <v>5</v>
       </c>
@@ -2961,7 +2961,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A47" t="s">
         <v>5</v>
       </c>
@@ -2984,7 +2984,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A48" t="s">
         <v>5</v>
       </c>
@@ -3007,7 +3007,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A49" t="s">
         <v>5</v>
       </c>
@@ -3030,7 +3030,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A50" t="s">
         <v>5</v>
       </c>
@@ -3053,7 +3053,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A51" t="s">
         <v>5</v>
       </c>
@@ -3076,7 +3076,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A52" t="s">
         <v>5</v>
       </c>
@@ -3099,7 +3099,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A53" t="s">
         <v>5</v>
       </c>
@@ -3122,7 +3122,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A54" t="s">
         <v>5</v>
       </c>
@@ -3145,7 +3145,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A55" t="s">
         <v>5</v>
       </c>
@@ -3168,7 +3168,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A56" t="s">
         <v>5</v>
       </c>
@@ -3191,7 +3191,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A57" t="s">
         <v>5</v>
       </c>
@@ -3214,7 +3214,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A58" t="s">
         <v>5</v>
       </c>
@@ -3237,7 +3237,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A59" t="s">
         <v>5</v>
       </c>
@@ -3260,7 +3260,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A60" t="s">
         <v>5</v>
       </c>
@@ -3283,7 +3283,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A61" t="s">
         <v>5</v>
       </c>
@@ -3306,7 +3306,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A62" t="s">
         <v>5</v>
       </c>
@@ -3329,7 +3329,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A63" t="s">
         <v>5</v>
       </c>
@@ -3352,7 +3352,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A64" t="s">
         <v>5</v>
       </c>
@@ -3375,7 +3375,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A65" t="s">
         <v>5</v>
       </c>
@@ -3398,7 +3398,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A66" t="s">
         <v>5</v>
       </c>
@@ -3421,7 +3421,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A67" t="s">
         <v>5</v>
       </c>
@@ -3444,7 +3444,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A68" t="s">
         <v>5</v>
       </c>
@@ -3467,7 +3467,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A69" t="s">
         <v>5</v>
       </c>
@@ -3490,7 +3490,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A70" t="s">
         <v>5</v>
       </c>
@@ -3513,7 +3513,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A71" t="s">
         <v>5</v>
       </c>
@@ -3536,7 +3536,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A72" t="s">
         <v>5</v>
       </c>
@@ -3559,7 +3559,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A73" t="s">
         <v>5</v>
       </c>
@@ -3582,7 +3582,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A74" t="s">
         <v>5</v>
       </c>
@@ -3605,7 +3605,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A75" t="s">
         <v>5</v>
       </c>
@@ -3628,7 +3628,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A76" t="s">
         <v>180</v>
       </c>
@@ -3651,7 +3651,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A77" t="s">
         <v>5</v>
       </c>
@@ -3674,7 +3674,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A78" t="s">
         <v>5</v>
       </c>
@@ -3697,7 +3697,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A79" t="s">
         <v>5</v>
       </c>
@@ -3720,7 +3720,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A80" t="s">
         <v>5</v>
       </c>
@@ -3743,7 +3743,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A81" t="s">
         <v>5</v>
       </c>
@@ -3766,7 +3766,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A82" t="s">
         <v>5</v>
       </c>
@@ -3789,7 +3789,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A83" t="s">
         <v>5</v>
       </c>
@@ -3812,7 +3812,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A84" t="s">
         <v>5</v>
       </c>
@@ -3835,7 +3835,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A85" t="s">
         <v>202</v>
       </c>
@@ -3858,7 +3858,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A86" t="s">
         <v>5</v>
       </c>
@@ -3881,7 +3881,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A87" t="s">
         <v>5</v>
       </c>
@@ -3904,7 +3904,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A88" t="s">
         <v>5</v>
       </c>
@@ -3927,7 +3927,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A89" t="s">
         <v>5</v>
       </c>
@@ -3950,14 +3950,14 @@
         <v>405</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A90" t="s">
         <v>5</v>
       </c>
       <c r="B90" t="s">
         <v>215</v>
       </c>
-      <c r="C90" s="2" t="s">
+      <c r="C90" s="3" t="s">
         <v>216</v>
       </c>
       <c r="D90" t="s">
@@ -3973,7 +3973,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A91" t="s">
         <v>5</v>
       </c>
@@ -3996,7 +3996,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A92" t="s">
         <v>5</v>
       </c>
@@ -4019,7 +4019,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A93" t="s">
         <v>5</v>
       </c>
@@ -4042,7 +4042,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A94" t="s">
         <v>5</v>
       </c>
@@ -4065,7 +4065,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A95" t="s">
         <v>5</v>
       </c>
@@ -4088,7 +4088,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A96" t="s">
         <v>5</v>
       </c>
@@ -4111,7 +4111,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A97" t="s">
         <v>5</v>
       </c>
@@ -4134,7 +4134,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A98" t="s">
         <v>5</v>
       </c>
@@ -4157,7 +4157,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A99" t="s">
         <v>5</v>
       </c>
@@ -4180,7 +4180,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A100" t="s">
         <v>5</v>
       </c>
@@ -4203,7 +4203,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A101" t="s">
         <v>5</v>
       </c>
@@ -4226,7 +4226,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A102" t="s">
         <v>5</v>
       </c>
@@ -4249,7 +4249,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A103" t="s">
         <v>5</v>
       </c>
@@ -4272,7 +4272,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A104" t="s">
         <v>5</v>
       </c>
@@ -4295,7 +4295,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A105" t="s">
         <v>5</v>
       </c>
@@ -4318,7 +4318,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A106" t="s">
         <v>5</v>
       </c>
@@ -4341,7 +4341,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A107" t="s">
         <v>5</v>
       </c>
@@ -4364,7 +4364,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A108" t="s">
         <v>5</v>
       </c>
@@ -4387,7 +4387,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A109" t="s">
         <v>5</v>
       </c>
@@ -4410,7 +4410,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A110" t="s">
         <v>5</v>
       </c>
@@ -4433,7 +4433,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A111" t="s">
         <v>5</v>
       </c>
@@ -4456,7 +4456,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A112" t="s">
         <v>5</v>
       </c>
@@ -4479,7 +4479,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A113" t="s">
         <v>5</v>
       </c>
@@ -4502,7 +4502,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A114" t="s">
         <v>5</v>
       </c>
@@ -4525,7 +4525,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A115" t="s">
         <v>5</v>
       </c>
@@ -4548,7 +4548,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A116" t="s">
         <v>5</v>
       </c>
@@ -4571,7 +4571,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A117" t="s">
         <v>5</v>
       </c>
@@ -4594,7 +4594,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A118" t="s">
         <v>5</v>
       </c>
@@ -4617,7 +4617,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A119" t="s">
         <v>5</v>
       </c>
@@ -4640,7 +4640,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A120" t="s">
         <v>5</v>
       </c>
@@ -4663,7 +4663,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A121" t="s">
         <v>5</v>
       </c>
@@ -4686,7 +4686,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A122" t="s">
         <v>5</v>
       </c>
@@ -4709,7 +4709,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A123" t="s">
         <v>5</v>
       </c>
@@ -4732,7 +4732,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A124" t="s">
         <v>5</v>
       </c>
@@ -4755,7 +4755,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A125" t="s">
         <v>5</v>
       </c>
@@ -4778,7 +4778,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A126" t="s">
         <v>5</v>
       </c>
@@ -4801,7 +4801,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A127" t="s">
         <v>5</v>
       </c>
@@ -4824,7 +4824,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A128" t="s">
         <v>5</v>
       </c>
@@ -4847,7 +4847,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="129" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A129" t="s">
         <v>5</v>
       </c>
@@ -4871,7 +4871,7 @@
       </c>
       <c r="V129" s="3"/>
     </row>
-    <row r="130" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A130" t="s">
         <v>5</v>
       </c>
@@ -4894,7 +4894,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="131" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A131" t="s">
         <v>5</v>
       </c>
@@ -4917,7 +4917,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="132" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A132" t="s">
         <v>5</v>
       </c>
@@ -4940,7 +4940,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="133" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A133" t="s">
         <v>5</v>
       </c>
@@ -4963,7 +4963,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="134" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A134" t="s">
         <v>5</v>
       </c>
@@ -4986,7 +4986,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="135" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A135" t="s">
         <v>5</v>
       </c>
@@ -5009,7 +5009,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="136" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A136" t="s">
         <v>5</v>
       </c>
@@ -5032,7 +5032,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="137" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A137" t="s">
         <v>5</v>
       </c>
@@ -5055,7 +5055,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="138" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A138" t="s">
         <v>5</v>
       </c>
@@ -5078,7 +5078,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="139" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A139" t="s">
         <v>5</v>
       </c>
@@ -5101,7 +5101,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="140" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A140" t="s">
         <v>5</v>
       </c>
@@ -5124,7 +5124,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="141" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A141" t="s">
         <v>5</v>
       </c>
@@ -5147,7 +5147,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="142" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A142" t="s">
         <v>5</v>
       </c>
@@ -5170,7 +5170,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="143" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A143" t="s">
         <v>5</v>
       </c>
@@ -5193,7 +5193,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="144" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A144" t="s">
         <v>5</v>
       </c>
@@ -5216,7 +5216,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A145" t="s">
         <v>5</v>
       </c>
@@ -5239,7 +5239,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A146" t="s">
         <v>5</v>
       </c>
@@ -5262,7 +5262,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A147" t="s">
         <v>5</v>
       </c>
@@ -5285,7 +5285,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A148" t="s">
         <v>5</v>
       </c>
@@ -5308,7 +5308,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A149" t="s">
         <v>5</v>
       </c>

</xml_diff>